<commit_message>
Modify tax scenario file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_TAX.xlsx
+++ b/SuppXLS/Scen_TRA_TAX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84630258-1D84-4E05-939F-2A0729952A5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42511D45-0197-4FAB-B5EA-393E86E8D957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2341,10 +2341,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AP10"/>
+  <dimension ref="B1:AP9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2437,20 +2437,20 @@
         <v>70</v>
       </c>
     </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+    </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="48" t="s">
+      <c r="B9" s="48" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="26" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{0D236EF8-9F91-4DE7-ABE4-EA7CDDB4332A}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{0D236EF8-9F91-4DE7-ABE4-EA7CDDB4332A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2459,10 +2459,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:L29"/>
+  <dimension ref="A2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2587,49 +2587,65 @@
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="41">
+        <f>'Tax Rate'!C87/1000</f>
+        <v>0.51367084945951402</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="14"/>
@@ -2639,12 +2655,12 @@
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="41">
-        <f>'Tax Rate'!C87/1000</f>
-        <v>0.51367084945951402</v>
+        <f>170/1000</f>
+        <v>0.17</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I20" s="14"/>
     </row>
@@ -2656,116 +2672,99 @@
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="41">
-        <f>170/1000</f>
-        <v>0.17</v>
+        <f>'Tax Rate'!C23/1000</f>
+        <v>0.12</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
         <v>78</v>
       </c>
       <c r="E22" s="14"/>
-      <c r="F22" s="41">
-        <f>'Tax Rate'!C23/1000</f>
-        <v>0.12</v>
+      <c r="F22" s="15">
+        <f>'Tax Rate'!C63/1000</f>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="20"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
       <c r="D23" s="14" t="s">
         <v>78</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="15">
-        <f>'Tax Rate'!C63/1000</f>
-        <v>6.7000000000000004E-2</v>
+        <f>'Tax Rate'!C61/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
       <c r="D24" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="14"/>
       <c r="F24" s="15">
-        <f>'Tax Rate'!C61/1000</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14" t="s">
-        <v>161</v>
+        <f>'Tax Rate'!C52/1000</f>
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="H24" t="s">
+        <v>162</v>
       </c>
       <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D25" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="15">
-        <f>'Tax Rate'!C52/1000</f>
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="H25" t="s">
-        <v>162</v>
-      </c>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="41">
+      <c r="F25" s="41">
         <f>AVERAGE('Tax Rate'!C53:C54)/1000</f>
         <v>0.46</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H25" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="42">
+      <c r="E26" s="16"/>
+      <c r="F26" s="42">
         <f>'Tax Rate'!C55/1000</f>
         <v>0.9</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F29" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2775,7 +2774,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="F26" formulaRange="1"/>
+    <ignoredError sqref="F25" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Modify registration tax for new cars
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_TAX.xlsx
+++ b/SuppXLS/Scen_TRA_TAX.xlsx
@@ -5,18 +5,19 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42511D45-0197-4FAB-B5EA-393E86E8D957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{42511D45-0197-4FAB-B5EA-393E86E8D957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5D94C3AD-94B7-4100-9A7B-0906A18F422B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="INS" sheetId="2" r:id="rId2"/>
-    <sheet name="UPD" sheetId="11" r:id="rId3"/>
-    <sheet name="Tax Rate" sheetId="16" r:id="rId4"/>
+    <sheet name="Filldata" sheetId="17" r:id="rId3"/>
+    <sheet name="UPD" sheetId="11" r:id="rId4"/>
+    <sheet name="Tax Rate" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="173">
   <si>
     <t>Year</t>
   </si>
@@ -607,6 +608,12 @@
   </si>
   <si>
     <t>* VRT is calculated as a percentage of the open market selling price (OMSP) of the vehicle. The average value is 14%.</t>
+  </si>
+  <si>
+    <t>T-CAR*</t>
+  </si>
+  <si>
+    <t>~TFM_Fill-R: w=INVCOST; Hcol=Region</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1063,7 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1145,6 +1152,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="5x indented GHG Textfiels" xfId="4" xr:uid="{5F614CE9-C529-4323-B893-6D57470EC2CB}"/>
@@ -2343,8 +2351,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AP9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2423,9 +2431,7 @@
       <c r="D5" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="44">
-        <v>2018</v>
-      </c>
+      <c r="E5" s="44"/>
       <c r="F5" s="47" t="s">
         <v>71</v>
       </c>
@@ -2457,12 +2463,207 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DAAC25-244F-41FD-BA97-CC0472A16D4A}">
+  <dimension ref="B3:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="14"/>
+      <c r="C4" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="14"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2779,7 +2980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA68FABB-07B7-4021-89BF-7BC43BCE1B04}">
   <dimension ref="B1:G95"/>
   <sheetViews>

</xml_diff>

<commit_message>
Edit tax scenario file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_TAX.xlsx
+++ b/SuppXLS/Scen_TRA_TAX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5D95C2-5475-496F-9A17-A0E06E0B20C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88AD068-3182-467E-80DF-FC4EBCE27E0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -9414,10 +9414,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AP91"/>
+  <dimension ref="A1:AP90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18:M19"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9441,7 +9441,7 @@
     <col min="43" max="43" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
@@ -9449,7 +9449,7 @@
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="46" t="s">
         <v>163</v>
       </c>
@@ -9469,7 +9469,7 @@
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B3" s="41" t="s">
         <v>154</v>
       </c>
@@ -9491,7 +9491,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>206</v>
       </c>
@@ -9509,7 +9509,7 @@
       <c r="S4" s="18"/>
       <c r="T4" s="18"/>
     </row>
-    <row r="5" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
@@ -9519,7 +9519,7 @@
       <c r="U5" s="17"/>
       <c r="V5" s="17"/>
     </row>
-    <row r="6" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="46" t="s">
         <v>208</v>
       </c>
@@ -9535,7 +9535,7 @@
       <c r="U6" s="17"/>
       <c r="V6" s="17"/>
     </row>
-    <row r="7" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>202</v>
       </c>
@@ -9551,7 +9551,7 @@
       <c r="U7" s="17"/>
       <c r="V7" s="17"/>
     </row>
-    <row r="8" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="41" t="s">
         <v>203</v>
       </c>
@@ -9567,7 +9567,7 @@
       <c r="U8" s="17"/>
       <c r="V8" s="17"/>
     </row>
-    <row r="9" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="50" t="s">
         <v>209</v>
       </c>
@@ -9580,7 +9580,7 @@
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
     </row>
-    <row r="10" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>73</v>
       </c>
@@ -9593,7 +9593,7 @@
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
     </row>
-    <row r="11" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>72</v>
       </c>
@@ -9606,7 +9606,7 @@
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
     </row>
-    <row r="12" spans="2:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="42"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
@@ -9617,9 +9617,9 @@
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -9629,482 +9629,498 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="4" t="str">
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="4" t="str">
         <f>INVCOST!B1</f>
         <v>attribute</v>
       </c>
-      <c r="C17" s="4" t="str">
+      <c r="C16" s="4" t="str">
         <f>INVCOST!C1</f>
         <v>process</v>
       </c>
-      <c r="D17" s="4" t="str">
+      <c r="D16" s="4" t="str">
         <f>INVCOST!D1</f>
         <v>commodity</v>
       </c>
-      <c r="E17" s="4" t="str">
+      <c r="E16" s="4" t="str">
         <f>INVCOST!E1</f>
         <v>lim_type</v>
       </c>
-      <c r="F17" s="4" t="str">
+      <c r="F16" s="4" t="str">
         <f>INVCOST!F1</f>
         <v>time_slice</v>
       </c>
-      <c r="G17" s="4" t="str">
+      <c r="G16" s="4" t="str">
         <f>INVCOST!G1</f>
         <v>year</v>
       </c>
-      <c r="H17" s="4" t="str">
+      <c r="H16" s="4" t="str">
         <f>INVCOST!H1</f>
         <v>commodity_group</v>
       </c>
-      <c r="I17" s="4" t="str">
+      <c r="I16" s="4" t="str">
         <f>INVCOST!I1</f>
         <v>currency</v>
       </c>
-      <c r="J17" s="4" t="str">
+      <c r="J16" s="4" t="str">
         <f>INVCOST!J1</f>
         <v>stage</v>
       </c>
-      <c r="K17" s="4" t="str">
+      <c r="K16" s="4" t="str">
         <f>INVCOST!K1</f>
         <v>sow</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="14" t="str">
+        <f>INVCOST!C2</f>
+        <v>T-CAR-BEV100_ELC21</v>
+      </c>
+      <c r="G17" s="14">
+        <f>INVCOST!G2</f>
+        <v>2018</v>
+      </c>
+      <c r="I17" s="14" t="str">
+        <f>INVCOST!I2</f>
+        <v>EUR18</v>
+      </c>
+      <c r="L17" s="44">
+        <f>INVCOST!L2*$C$3+IF(NOT(ISERR(FIND($B$8,C17))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C17))),$C$7,0)</f>
+        <v>32.586939999999991</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C18" s="14" t="str">
-        <f>INVCOST!C2</f>
+        <f>INVCOST!C3</f>
         <v>T-CAR-BEV100_ELC21</v>
       </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="14">
-        <f>INVCOST!G2</f>
-        <v>2018</v>
-      </c>
+        <f>INVCOST!G3</f>
+        <v>2030</v>
+      </c>
+      <c r="H18" s="14"/>
       <c r="I18" s="14" t="str">
-        <f>INVCOST!I2</f>
+        <f>INVCOST!I3</f>
         <v>EUR18</v>
       </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="44">
-        <f>INVCOST!L2*$C$3+IF(NOT(ISERR(FIND($B$8,C18))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C18))),$C$7,0)</f>
-        <v>32.586939999999991</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <f>INVCOST!L3*$C$3+IF(NOT(ISERR(FIND($B$8,C18))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C18))),$C$7,0)</f>
+        <v>26.442339999999998</v>
+      </c>
+      <c r="O18" s="14"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C19" s="14" t="str">
-        <f>INVCOST!C3</f>
+        <f>INVCOST!C4</f>
         <v>T-CAR-BEV100_ELC21</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14">
-        <f>INVCOST!G3</f>
-        <v>2030</v>
+        <f>INVCOST!G4</f>
+        <v>2050</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14" t="str">
-        <f>INVCOST!I3</f>
+        <f>INVCOST!I4</f>
         <v>EUR18</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="44">
-        <f>INVCOST!L3*$C$3+IF(NOT(ISERR(FIND($B$8,C19))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C19))),$C$7,0)</f>
-        <v>26.442339999999998</v>
+        <f>INVCOST!L4*$C$3+IF(NOT(ISERR(FIND($B$8,C19))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C19))),$C$7,0)</f>
+        <v>23.096439999999998</v>
       </c>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C20" s="14" t="str">
-        <f>INVCOST!C4</f>
-        <v>T-CAR-BEV100_ELC21</v>
+        <f>INVCOST!C5</f>
+        <v>T-CAR-BEV150_ELC21</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14">
-        <f>INVCOST!G4</f>
-        <v>2050</v>
+        <f>INVCOST!G5</f>
+        <v>2018</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="str">
-        <f>INVCOST!I4</f>
+        <f>INVCOST!I5</f>
         <v>EUR18</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="44">
-        <f>INVCOST!L4*$C$3+IF(NOT(ISERR(FIND($B$8,C20))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C20))),$C$7,0)</f>
-        <v>23.096439999999998</v>
+        <f>INVCOST!L5*$C$3+IF(NOT(ISERR(FIND($B$8,C20))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C20))),$C$7,0)</f>
+        <v>32.586939999999991</v>
       </c>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C21" s="14" t="str">
-        <f>INVCOST!C5</f>
+        <f>INVCOST!C6</f>
         <v>T-CAR-BEV150_ELC21</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14">
-        <f>INVCOST!G5</f>
-        <v>2018</v>
+        <f>INVCOST!G6</f>
+        <v>2030</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="str">
-        <f>INVCOST!I5</f>
+        <f>INVCOST!I6</f>
         <v>EUR18</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="44">
-        <f>INVCOST!L5*$C$3+IF(NOT(ISERR(FIND($B$8,C21))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C21))),$C$7,0)</f>
-        <v>32.586939999999991</v>
+        <f>INVCOST!L6*$C$3+IF(NOT(ISERR(FIND($B$8,C21))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C21))),$C$7,0)</f>
+        <v>26.442339999999998</v>
       </c>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C22" s="14" t="str">
-        <f>INVCOST!C6</f>
+        <f>INVCOST!C7</f>
         <v>T-CAR-BEV150_ELC21</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14">
-        <f>INVCOST!G6</f>
-        <v>2030</v>
+        <f>INVCOST!G7</f>
+        <v>2050</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14" t="str">
-        <f>INVCOST!I6</f>
+        <f>INVCOST!I7</f>
         <v>EUR18</v>
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="44">
-        <f>INVCOST!L6*$C$3+IF(NOT(ISERR(FIND($B$8,C22))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C22))),$C$7,0)</f>
-        <v>26.442339999999998</v>
+        <f>INVCOST!L7*$C$3+IF(NOT(ISERR(FIND($B$8,C22))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C22))),$C$7,0)</f>
+        <v>23.096439999999998</v>
       </c>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C23" s="14" t="str">
-        <f>INVCOST!C7</f>
-        <v>T-CAR-BEV150_ELC21</v>
+        <f>INVCOST!C8</f>
+        <v>T-CAR-BEV250_ELC21</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14">
-        <f>INVCOST!G7</f>
-        <v>2050</v>
+        <f>INVCOST!G8</f>
+        <v>2018</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="str">
-        <f>INVCOST!I7</f>
+        <f>INVCOST!I8</f>
         <v>EUR18</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="44">
-        <f>INVCOST!L7*$C$3+IF(NOT(ISERR(FIND($B$8,C23))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C23))),$C$7,0)</f>
-        <v>23.096439999999998</v>
+        <f>INVCOST!L8*$C$3+IF(NOT(ISERR(FIND($B$8,C23))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C23))),$C$7,0)</f>
+        <v>32.586939999999991</v>
       </c>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C24" s="14" t="str">
-        <f>INVCOST!C8</f>
+        <f>INVCOST!C9</f>
         <v>T-CAR-BEV250_ELC21</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14">
-        <f>INVCOST!G8</f>
-        <v>2018</v>
+        <f>INVCOST!G9</f>
+        <v>2030</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14" t="str">
-        <f>INVCOST!I8</f>
+        <f>INVCOST!I9</f>
         <v>EUR18</v>
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
       <c r="L24" s="44">
-        <f>INVCOST!L8*$C$3+IF(NOT(ISERR(FIND($B$8,C24))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C24))),$C$7,0)</f>
-        <v>32.586939999999991</v>
+        <f>INVCOST!L9*$C$3+IF(NOT(ISERR(FIND($B$8,C24))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C24))),$C$7,0)</f>
+        <v>26.442339999999998</v>
       </c>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C25" s="14" t="str">
-        <f>INVCOST!C9</f>
+        <f>INVCOST!C10</f>
         <v>T-CAR-BEV250_ELC21</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14">
-        <f>INVCOST!G9</f>
-        <v>2030</v>
+        <f>INVCOST!G10</f>
+        <v>2050</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14" t="str">
-        <f>INVCOST!I9</f>
+        <f>INVCOST!I10</f>
         <v>EUR18</v>
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="44">
-        <f>INVCOST!L9*$C$3+IF(NOT(ISERR(FIND($B$8,C25))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C25))),$C$7,0)</f>
-        <v>26.442339999999998</v>
+        <f>INVCOST!L10*$C$3+IF(NOT(ISERR(FIND($B$8,C25))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C25))),$C$7,0)</f>
+        <v>23.096439999999998</v>
       </c>
       <c r="O25" s="14"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C26" s="14" t="str">
-        <f>INVCOST!C10</f>
-        <v>T-CAR-BEV250_ELC21</v>
+        <f>INVCOST!C11</f>
+        <v>T-CAR-FCV_HYD21</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14">
-        <f>INVCOST!G10</f>
-        <v>2050</v>
+        <f>INVCOST!G11</f>
+        <v>2018</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="14" t="str">
-        <f>INVCOST!I10</f>
+        <f>INVCOST!I11</f>
         <v>EUR18</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
       <c r="L26" s="44">
-        <f>INVCOST!L10*$C$3+IF(NOT(ISERR(FIND($B$8,C26))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C26))),$C$7,0)</f>
-        <v>23.096439999999998</v>
+        <f>INVCOST!L11*$C$3+IF(NOT(ISERR(FIND($B$8,C26))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C26))),$C$7,0)</f>
+        <v>69.333659999999995</v>
       </c>
       <c r="O26" s="14"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C27" s="14" t="str">
-        <f>INVCOST!C11</f>
+        <f>INVCOST!C12</f>
         <v>T-CAR-FCV_HYD21</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14">
-        <f>INVCOST!G11</f>
-        <v>2018</v>
+        <f>INVCOST!G12</f>
+        <v>2030</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="14" t="str">
-        <f>INVCOST!I11</f>
+        <f>INVCOST!I12</f>
         <v>EUR18</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
       <c r="L27" s="44">
-        <f>INVCOST!L11*$C$3+IF(NOT(ISERR(FIND($B$8,C27))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C27))),$C$7,0)</f>
-        <v>69.333659999999995</v>
+        <f>INVCOST!L12*$C$3+IF(NOT(ISERR(FIND($B$8,C27))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C27))),$C$7,0)</f>
+        <v>35.549759999999999</v>
       </c>
       <c r="O27" s="14"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C28" s="14" t="str">
-        <f>INVCOST!C12</f>
+        <f>INVCOST!C13</f>
         <v>T-CAR-FCV_HYD21</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14">
-        <f>INVCOST!G12</f>
-        <v>2030</v>
+        <f>INVCOST!G13</f>
+        <v>2050</v>
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="14" t="str">
-        <f>INVCOST!I12</f>
+        <f>INVCOST!I13</f>
         <v>EUR18</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="44">
-        <f>INVCOST!L12*$C$3+IF(NOT(ISERR(FIND($B$8,C28))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C28))),$C$7,0)</f>
-        <v>35.549759999999999</v>
+        <f>INVCOST!L13*$C$3+IF(NOT(ISERR(FIND($B$8,C28))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C28))),$C$7,0)</f>
+        <v>28.267439999999997</v>
       </c>
       <c r="O28" s="14"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C29" s="14" t="str">
-        <f>INVCOST!C13</f>
-        <v>T-CAR-FCV_HYD21</v>
+        <f>INVCOST!C14</f>
+        <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14">
-        <f>INVCOST!G13</f>
-        <v>2050</v>
+        <f>INVCOST!G14</f>
+        <v>2018</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14" t="str">
-        <f>INVCOST!I13</f>
+        <f>INVCOST!I14</f>
         <v>EUR18</v>
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="44">
-        <f>INVCOST!L13*$C$3+IF(NOT(ISERR(FIND($B$8,C29))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C29))),$C$7,0)</f>
-        <v>28.267439999999997</v>
+        <f>INVCOST!L14*$C$3+IF(NOT(ISERR(FIND($B$8,C29))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C29))),$C$7,0)</f>
+        <v>29.236439999999998</v>
       </c>
       <c r="O29" s="14"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C30" s="14" t="str">
-        <f>INVCOST!C14</f>
+        <f>INVCOST!C15</f>
         <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14">
-        <f>INVCOST!G14</f>
-        <v>2018</v>
+        <f>INVCOST!G15</f>
+        <v>2030</v>
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="14" t="str">
-        <f>INVCOST!I14</f>
+        <f>INVCOST!I15</f>
         <v>EUR18</v>
       </c>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
       <c r="L30" s="44">
-        <f>INVCOST!L14*$C$3+IF(NOT(ISERR(FIND($B$8,C30))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C30))),$C$7,0)</f>
-        <v>29.236439999999998</v>
+        <f>INVCOST!L15*$C$3+IF(NOT(ISERR(FIND($B$8,C30))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C30))),$C$7,0)</f>
+        <v>28.87848</v>
       </c>
       <c r="O30" s="14"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C31" s="14" t="str">
-        <f>INVCOST!C15</f>
+        <f>INVCOST!C16</f>
         <v>T-CAR-HEV_DST21</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14">
-        <f>INVCOST!G15</f>
-        <v>2030</v>
+        <f>INVCOST!G16</f>
+        <v>2050</v>
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="14" t="str">
-        <f>INVCOST!I15</f>
+        <f>INVCOST!I16</f>
         <v>EUR18</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
       <c r="L31" s="44">
-        <f>INVCOST!L15*$C$3+IF(NOT(ISERR(FIND($B$8,C31))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C31))),$C$7,0)</f>
-        <v>28.87848</v>
+        <f>INVCOST!L16*$C$3+IF(NOT(ISERR(FIND($B$8,C31))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C31))),$C$7,0)</f>
+        <v>28.008659999999995</v>
       </c>
       <c r="O31" s="14"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
         <v>177</v>
       </c>
       <c r="C32" s="14" t="str">
-        <f>INVCOST!C16</f>
-        <v>T-CAR-HEV_DST21</v>
+        <f>INVCOST!C17</f>
+        <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14">
-        <f>INVCOST!G16</f>
-        <v>2050</v>
+        <f>INVCOST!G17</f>
+        <v>2018</v>
       </c>
       <c r="H32" s="14"/>
       <c r="I32" s="14" t="str">
-        <f>INVCOST!I16</f>
+        <f>INVCOST!I17</f>
         <v>EUR18</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="44">
-        <f>INVCOST!L16*$C$3+IF(NOT(ISERR(FIND($B$8,C32))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C32))),$C$7,0)</f>
-        <v>28.008659999999995</v>
+        <f>INVCOST!L17*$C$3+IF(NOT(ISERR(FIND($B$8,C32))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C32))),$C$7,0)</f>
+        <v>27.077279999999995</v>
       </c>
       <c r="O32" s="14"/>
     </row>
@@ -10113,26 +10129,26 @@
         <v>177</v>
       </c>
       <c r="C33" s="14" t="str">
-        <f>INVCOST!C17</f>
+        <f>INVCOST!C18</f>
         <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14">
-        <f>INVCOST!G17</f>
-        <v>2018</v>
+        <f>INVCOST!G18</f>
+        <v>2030</v>
       </c>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="str">
-        <f>INVCOST!I17</f>
+        <f>INVCOST!I18</f>
         <v>EUR18</v>
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
       <c r="L33" s="44">
-        <f>INVCOST!L17*$C$3+IF(NOT(ISERR(FIND($B$8,C33))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C33))),$C$7,0)</f>
-        <v>27.077279999999995</v>
+        <f>INVCOST!L18*$C$3+IF(NOT(ISERR(FIND($B$8,C33))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C33))),$C$7,0)</f>
+        <v>26.762639999999998</v>
       </c>
       <c r="O33" s="14"/>
     </row>
@@ -10141,26 +10157,26 @@
         <v>177</v>
       </c>
       <c r="C34" s="14" t="str">
-        <f>INVCOST!C18</f>
+        <f>INVCOST!C19</f>
         <v>T-CAR-HEV_GSL21</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14">
-        <f>INVCOST!G18</f>
-        <v>2030</v>
+        <f>INVCOST!G19</f>
+        <v>2050</v>
       </c>
       <c r="H34" s="14"/>
       <c r="I34" s="14" t="str">
-        <f>INVCOST!I18</f>
+        <f>INVCOST!I19</f>
         <v>EUR18</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
       <c r="L34" s="44">
-        <f>INVCOST!L18*$C$3+IF(NOT(ISERR(FIND($B$8,C34))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C34))),$C$7,0)</f>
-        <v>26.762639999999998</v>
+        <f>INVCOST!L19*$C$3+IF(NOT(ISERR(FIND($B$8,C34))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C34))),$C$7,0)</f>
+        <v>25.956659999999996</v>
       </c>
       <c r="O34" s="14"/>
     </row>
@@ -10169,26 +10185,26 @@
         <v>177</v>
       </c>
       <c r="C35" s="14" t="str">
-        <f>INVCOST!C19</f>
-        <v>T-CAR-HEV_GSL21</v>
+        <f>INVCOST!C20</f>
+        <v>T-CAR-ICE_B10021</v>
       </c>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14">
-        <f>INVCOST!G19</f>
-        <v>2050</v>
+        <f>INVCOST!G20</f>
+        <v>2018</v>
       </c>
       <c r="H35" s="14"/>
       <c r="I35" s="14" t="str">
-        <f>INVCOST!I19</f>
+        <f>INVCOST!I20</f>
         <v>EUR18</v>
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
       <c r="L35" s="44">
-        <f>INVCOST!L19*$C$3+IF(NOT(ISERR(FIND($B$8,C35))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C35))),$C$7,0)</f>
-        <v>25.956659999999996</v>
+        <f>INVCOST!L20*$C$3+IF(NOT(ISERR(FIND($B$8,C35))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C35))),$C$7,0)</f>
+        <v>24.888009274342181</v>
       </c>
       <c r="O35" s="14"/>
     </row>
@@ -10197,25 +10213,25 @@
         <v>177</v>
       </c>
       <c r="C36" s="14" t="str">
-        <f>INVCOST!C20</f>
+        <f>INVCOST!C21</f>
         <v>T-CAR-ICE_B10021</v>
       </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14">
-        <f>INVCOST!G20</f>
-        <v>2018</v>
+        <f>INVCOST!G21</f>
+        <v>2030</v>
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="14" t="str">
-        <f>INVCOST!I20</f>
+        <f>INVCOST!I21</f>
         <v>EUR18</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
       <c r="L36" s="44">
-        <f>INVCOST!L20*$C$3+IF(NOT(ISERR(FIND($B$8,C36))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C36))),$C$7,0)</f>
+        <f>INVCOST!L21*$C$3+IF(NOT(ISERR(FIND($B$8,C36))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C36))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O36" s="14"/>
@@ -10225,25 +10241,25 @@
         <v>177</v>
       </c>
       <c r="C37" s="14" t="str">
-        <f>INVCOST!C21</f>
+        <f>INVCOST!C22</f>
         <v>T-CAR-ICE_B10021</v>
       </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14">
-        <f>INVCOST!G21</f>
-        <v>2030</v>
+        <f>INVCOST!G22</f>
+        <v>2050</v>
       </c>
       <c r="H37" s="14"/>
       <c r="I37" s="14" t="str">
-        <f>INVCOST!I21</f>
+        <f>INVCOST!I22</f>
         <v>EUR18</v>
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
       <c r="L37" s="44">
-        <f>INVCOST!L21*$C$3+IF(NOT(ISERR(FIND($B$8,C37))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C37))),$C$7,0)</f>
+        <f>INVCOST!L22*$C$3+IF(NOT(ISERR(FIND($B$8,C37))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C37))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O37" s="14"/>
@@ -10253,25 +10269,25 @@
         <v>177</v>
       </c>
       <c r="C38" s="14" t="str">
-        <f>INVCOST!C22</f>
-        <v>T-CAR-ICE_B10021</v>
+        <f>INVCOST!C23</f>
+        <v>T-CAR-ICE_DF21</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14">
-        <f>INVCOST!G22</f>
-        <v>2050</v>
+        <f>INVCOST!G23</f>
+        <v>2018</v>
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="14" t="str">
-        <f>INVCOST!I22</f>
+        <f>INVCOST!I23</f>
         <v>EUR18</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
       <c r="L38" s="44">
-        <f>INVCOST!L22*$C$3+IF(NOT(ISERR(FIND($B$8,C38))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C38))),$C$7,0)</f>
+        <f>INVCOST!L23*$C$3+IF(NOT(ISERR(FIND($B$8,C38))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C38))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O38" s="14"/>
@@ -10281,25 +10297,25 @@
         <v>177</v>
       </c>
       <c r="C39" s="14" t="str">
-        <f>INVCOST!C23</f>
+        <f>INVCOST!C24</f>
         <v>T-CAR-ICE_DF21</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14">
-        <f>INVCOST!G23</f>
-        <v>2018</v>
+        <f>INVCOST!G24</f>
+        <v>2030</v>
       </c>
       <c r="H39" s="14"/>
       <c r="I39" s="14" t="str">
-        <f>INVCOST!I23</f>
+        <f>INVCOST!I24</f>
         <v>EUR18</v>
       </c>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
       <c r="L39" s="44">
-        <f>INVCOST!L23*$C$3+IF(NOT(ISERR(FIND($B$8,C39))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C39))),$C$7,0)</f>
+        <f>INVCOST!L24*$C$3+IF(NOT(ISERR(FIND($B$8,C39))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C39))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O39" s="14"/>
@@ -10309,25 +10325,25 @@
         <v>177</v>
       </c>
       <c r="C40" s="14" t="str">
-        <f>INVCOST!C24</f>
+        <f>INVCOST!C25</f>
         <v>T-CAR-ICE_DF21</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="14">
-        <f>INVCOST!G24</f>
-        <v>2030</v>
+        <f>INVCOST!G25</f>
+        <v>2050</v>
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14" t="str">
-        <f>INVCOST!I24</f>
+        <f>INVCOST!I25</f>
         <v>EUR18</v>
       </c>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
       <c r="L40" s="44">
-        <f>INVCOST!L24*$C$3+IF(NOT(ISERR(FIND($B$8,C40))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C40))),$C$7,0)</f>
+        <f>INVCOST!L25*$C$3+IF(NOT(ISERR(FIND($B$8,C40))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C40))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O40" s="14"/>
@@ -10337,25 +10353,25 @@
         <v>177</v>
       </c>
       <c r="C41" s="14" t="str">
-        <f>INVCOST!C25</f>
-        <v>T-CAR-ICE_DF21</v>
+        <f>INVCOST!C26</f>
+        <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14">
-        <f>INVCOST!G25</f>
-        <v>2050</v>
+        <f>INVCOST!G26</f>
+        <v>2018</v>
       </c>
       <c r="H41" s="14"/>
       <c r="I41" s="14" t="str">
-        <f>INVCOST!I25</f>
+        <f>INVCOST!I26</f>
         <v>EUR18</v>
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
       <c r="L41" s="44">
-        <f>INVCOST!L25*$C$3+IF(NOT(ISERR(FIND($B$8,C41))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C41))),$C$7,0)</f>
+        <f>INVCOST!L26*$C$3+IF(NOT(ISERR(FIND($B$8,C41))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C41))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O41" s="14"/>
@@ -10365,25 +10381,25 @@
         <v>177</v>
       </c>
       <c r="C42" s="14" t="str">
-        <f>INVCOST!C26</f>
+        <f>INVCOST!C27</f>
         <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14">
-        <f>INVCOST!G26</f>
-        <v>2018</v>
+        <f>INVCOST!G27</f>
+        <v>2030</v>
       </c>
       <c r="H42" s="14"/>
       <c r="I42" s="14" t="str">
-        <f>INVCOST!I26</f>
+        <f>INVCOST!I27</f>
         <v>EUR18</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
       <c r="L42" s="44">
-        <f>INVCOST!L26*$C$3+IF(NOT(ISERR(FIND($B$8,C42))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C42))),$C$7,0)</f>
+        <f>INVCOST!L27*$C$3+IF(NOT(ISERR(FIND($B$8,C42))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C42))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O42" s="14"/>
@@ -10393,25 +10409,25 @@
         <v>177</v>
       </c>
       <c r="C43" s="14" t="str">
-        <f>INVCOST!C27</f>
+        <f>INVCOST!C28</f>
         <v>T-CAR-ICE_DST21</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14">
-        <f>INVCOST!G27</f>
-        <v>2030</v>
+        <f>INVCOST!G28</f>
+        <v>2050</v>
       </c>
       <c r="H43" s="14"/>
       <c r="I43" s="14" t="str">
-        <f>INVCOST!I27</f>
+        <f>INVCOST!I28</f>
         <v>EUR18</v>
       </c>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="44">
-        <f>INVCOST!L27*$C$3+IF(NOT(ISERR(FIND($B$8,C43))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C43))),$C$7,0)</f>
+        <f>INVCOST!L28*$C$3+IF(NOT(ISERR(FIND($B$8,C43))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C43))),$C$7,0)</f>
         <v>24.888009274342181</v>
       </c>
       <c r="O43" s="14"/>
@@ -10421,26 +10437,26 @@
         <v>177</v>
       </c>
       <c r="C44" s="14" t="str">
-        <f>INVCOST!C28</f>
-        <v>T-CAR-ICE_DST21</v>
+        <f>INVCOST!C29</f>
+        <v>T-CAR-ICE_E8521</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14">
-        <f>INVCOST!G28</f>
-        <v>2050</v>
+        <f>INVCOST!G29</f>
+        <v>2018</v>
       </c>
       <c r="H44" s="14"/>
       <c r="I44" s="14" t="str">
-        <f>INVCOST!I28</f>
+        <f>INVCOST!I29</f>
         <v>EUR18</v>
       </c>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="44">
-        <f>INVCOST!L28*$C$3+IF(NOT(ISERR(FIND($B$8,C44))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C44))),$C$7,0)</f>
-        <v>24.888009274342181</v>
+        <f>INVCOST!L29*$C$3+IF(NOT(ISERR(FIND($B$8,C44))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C44))),$C$7,0)</f>
+        <v>23.130765053247</v>
       </c>
       <c r="O44" s="14"/>
     </row>
@@ -10449,25 +10465,25 @@
         <v>177</v>
       </c>
       <c r="C45" s="14" t="str">
-        <f>INVCOST!C29</f>
+        <f>INVCOST!C30</f>
         <v>T-CAR-ICE_E8521</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14">
-        <f>INVCOST!G29</f>
-        <v>2018</v>
+        <f>INVCOST!G30</f>
+        <v>2030</v>
       </c>
       <c r="H45" s="14"/>
       <c r="I45" s="14" t="str">
-        <f>INVCOST!I29</f>
+        <f>INVCOST!I30</f>
         <v>EUR18</v>
       </c>
       <c r="J45" s="14"/>
       <c r="K45" s="14"/>
       <c r="L45" s="44">
-        <f>INVCOST!L29*$C$3+IF(NOT(ISERR(FIND($B$8,C45))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C45))),$C$7,0)</f>
+        <f>INVCOST!L30*$C$3+IF(NOT(ISERR(FIND($B$8,C45))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C45))),$C$7,0)</f>
         <v>23.130765053247</v>
       </c>
       <c r="O45" s="14"/>
@@ -10477,25 +10493,25 @@
         <v>177</v>
       </c>
       <c r="C46" s="14" t="str">
-        <f>INVCOST!C30</f>
+        <f>INVCOST!C31</f>
         <v>T-CAR-ICE_E8521</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14">
-        <f>INVCOST!G30</f>
-        <v>2030</v>
+        <f>INVCOST!G31</f>
+        <v>2050</v>
       </c>
       <c r="H46" s="14"/>
       <c r="I46" s="14" t="str">
-        <f>INVCOST!I30</f>
+        <f>INVCOST!I31</f>
         <v>EUR18</v>
       </c>
       <c r="J46" s="14"/>
       <c r="K46" s="14"/>
       <c r="L46" s="44">
-        <f>INVCOST!L30*$C$3+IF(NOT(ISERR(FIND($B$8,C46))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C46))),$C$7,0)</f>
+        <f>INVCOST!L31*$C$3+IF(NOT(ISERR(FIND($B$8,C46))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C46))),$C$7,0)</f>
         <v>23.130765053247</v>
       </c>
       <c r="O46" s="14"/>
@@ -10505,25 +10521,25 @@
         <v>177</v>
       </c>
       <c r="C47" s="14" t="str">
-        <f>INVCOST!C31</f>
-        <v>T-CAR-ICE_E8521</v>
+        <f>INVCOST!C32</f>
+        <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
       <c r="G47" s="14">
-        <f>INVCOST!G31</f>
-        <v>2050</v>
+        <f>INVCOST!G32</f>
+        <v>2018</v>
       </c>
       <c r="H47" s="14"/>
       <c r="I47" s="14" t="str">
-        <f>INVCOST!I31</f>
+        <f>INVCOST!I32</f>
         <v>EUR18</v>
       </c>
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
       <c r="L47" s="44">
-        <f>INVCOST!L31*$C$3+IF(NOT(ISERR(FIND($B$8,C47))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C47))),$C$7,0)</f>
+        <f>INVCOST!L32*$C$3+IF(NOT(ISERR(FIND($B$8,C47))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C47))),$C$7,0)</f>
         <v>23.130765053247</v>
       </c>
       <c r="O47" s="14"/>
@@ -10533,25 +10549,25 @@
         <v>177</v>
       </c>
       <c r="C48" s="14" t="str">
-        <f>INVCOST!C32</f>
+        <f>INVCOST!C33</f>
         <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="G48" s="14">
-        <f>INVCOST!G32</f>
-        <v>2018</v>
+        <f>INVCOST!G33</f>
+        <v>2030</v>
       </c>
       <c r="H48" s="14"/>
       <c r="I48" s="14" t="str">
-        <f>INVCOST!I32</f>
+        <f>INVCOST!I33</f>
         <v>EUR18</v>
       </c>
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
       <c r="L48" s="44">
-        <f>INVCOST!L32*$C$3+IF(NOT(ISERR(FIND($B$8,C48))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C48))),$C$7,0)</f>
+        <f>INVCOST!L33*$C$3+IF(NOT(ISERR(FIND($B$8,C48))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C48))),$C$7,0)</f>
         <v>23.130765053247</v>
       </c>
       <c r="O48" s="14"/>
@@ -10561,25 +10577,25 @@
         <v>177</v>
       </c>
       <c r="C49" s="14" t="str">
-        <f>INVCOST!C33</f>
+        <f>INVCOST!C34</f>
         <v>T-CAR-ICE_GSL21</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14">
-        <f>INVCOST!G33</f>
-        <v>2030</v>
+        <f>INVCOST!G34</f>
+        <v>2050</v>
       </c>
       <c r="H49" s="14"/>
       <c r="I49" s="14" t="str">
-        <f>INVCOST!I33</f>
+        <f>INVCOST!I34</f>
         <v>EUR18</v>
       </c>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
       <c r="L49" s="44">
-        <f>INVCOST!L33*$C$3+IF(NOT(ISERR(FIND($B$8,C49))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C49))),$C$7,0)</f>
+        <f>INVCOST!L34*$C$3+IF(NOT(ISERR(FIND($B$8,C49))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C49))),$C$7,0)</f>
         <v>23.130765053247</v>
       </c>
       <c r="O49" s="14"/>
@@ -10589,26 +10605,26 @@
         <v>177</v>
       </c>
       <c r="C50" s="14" t="str">
-        <f>INVCOST!C34</f>
-        <v>T-CAR-ICE_GSL21</v>
+        <f>INVCOST!C35</f>
+        <v>T-CAR-ICE_HYD21</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14">
-        <f>INVCOST!G34</f>
-        <v>2050</v>
+        <f>INVCOST!G35</f>
+        <v>2018</v>
       </c>
       <c r="H50" s="14"/>
       <c r="I50" s="14" t="str">
-        <f>INVCOST!I34</f>
+        <f>INVCOST!I35</f>
         <v>EUR18</v>
       </c>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
       <c r="L50" s="44">
-        <f>INVCOST!L34*$C$3+IF(NOT(ISERR(FIND($B$8,C50))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C50))),$C$7,0)</f>
-        <v>23.130765053247</v>
+        <f>INVCOST!L35*$C$3+IF(NOT(ISERR(FIND($B$8,C50))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C50))),$C$7,0)</f>
+        <v>69.333659999999995</v>
       </c>
       <c r="O50" s="14"/>
     </row>
@@ -10617,26 +10633,26 @@
         <v>177</v>
       </c>
       <c r="C51" s="14" t="str">
-        <f>INVCOST!C35</f>
+        <f>INVCOST!C36</f>
         <v>T-CAR-ICE_HYD21</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
       <c r="G51" s="14">
-        <f>INVCOST!G35</f>
-        <v>2018</v>
+        <f>INVCOST!G36</f>
+        <v>2030</v>
       </c>
       <c r="H51" s="14"/>
       <c r="I51" s="14" t="str">
-        <f>INVCOST!I35</f>
+        <f>INVCOST!I36</f>
         <v>EUR18</v>
       </c>
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
       <c r="L51" s="44">
-        <f>INVCOST!L35*$C$3+IF(NOT(ISERR(FIND($B$8,C51))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C51))),$C$7,0)</f>
-        <v>69.333659999999995</v>
+        <f>INVCOST!L36*$C$3+IF(NOT(ISERR(FIND($B$8,C51))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C51))),$C$7,0)</f>
+        <v>35.549759999999999</v>
       </c>
       <c r="O51" s="14"/>
     </row>
@@ -10645,26 +10661,26 @@
         <v>177</v>
       </c>
       <c r="C52" s="14" t="str">
-        <f>INVCOST!C36</f>
+        <f>INVCOST!C37</f>
         <v>T-CAR-ICE_HYD21</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
       <c r="G52" s="14">
-        <f>INVCOST!G36</f>
-        <v>2030</v>
+        <f>INVCOST!G37</f>
+        <v>2050</v>
       </c>
       <c r="H52" s="14"/>
       <c r="I52" s="14" t="str">
-        <f>INVCOST!I36</f>
+        <f>INVCOST!I37</f>
         <v>EUR18</v>
       </c>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
       <c r="L52" s="44">
-        <f>INVCOST!L36*$C$3+IF(NOT(ISERR(FIND($B$8,C52))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C52))),$C$7,0)</f>
-        <v>35.549759999999999</v>
+        <f>INVCOST!L37*$C$3+IF(NOT(ISERR(FIND($B$8,C52))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C52))),$C$7,0)</f>
+        <v>28.267439999999997</v>
       </c>
       <c r="O52" s="14"/>
     </row>
@@ -10673,26 +10689,26 @@
         <v>177</v>
       </c>
       <c r="C53" s="14" t="str">
-        <f>INVCOST!C37</f>
-        <v>T-CAR-ICE_HYD21</v>
+        <f>INVCOST!C38</f>
+        <v>T-CAR-ICE_NGB21</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
       <c r="G53" s="14">
-        <f>INVCOST!G37</f>
-        <v>2050</v>
+        <f>INVCOST!G38</f>
+        <v>2018</v>
       </c>
       <c r="H53" s="14"/>
       <c r="I53" s="14" t="str">
-        <f>INVCOST!I37</f>
+        <f>INVCOST!I38</f>
         <v>EUR18</v>
       </c>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
       <c r="L53" s="44">
-        <f>INVCOST!L37*$C$3+IF(NOT(ISERR(FIND($B$8,C53))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C53))),$C$7,0)</f>
-        <v>28.267439999999997</v>
+        <f>INVCOST!L38*$C$3+IF(NOT(ISERR(FIND($B$8,C53))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C53))),$C$7,0)</f>
+        <v>28.079339999999998</v>
       </c>
       <c r="O53" s="14"/>
     </row>
@@ -10701,25 +10717,25 @@
         <v>177</v>
       </c>
       <c r="C54" s="14" t="str">
-        <f>INVCOST!C38</f>
+        <f>INVCOST!C39</f>
         <v>T-CAR-ICE_NGB21</v>
       </c>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14">
-        <f>INVCOST!G38</f>
-        <v>2018</v>
+        <f>INVCOST!G39</f>
+        <v>2030</v>
       </c>
       <c r="H54" s="14"/>
       <c r="I54" s="14" t="str">
-        <f>INVCOST!I38</f>
+        <f>INVCOST!I39</f>
         <v>EUR18</v>
       </c>
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
       <c r="L54" s="44">
-        <f>INVCOST!L38*$C$3+IF(NOT(ISERR(FIND($B$8,C54))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C54))),$C$7,0)</f>
+        <f>INVCOST!L39*$C$3+IF(NOT(ISERR(FIND($B$8,C54))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C54))),$C$7,0)</f>
         <v>28.079339999999998</v>
       </c>
       <c r="O54" s="14"/>
@@ -10729,25 +10745,25 @@
         <v>177</v>
       </c>
       <c r="C55" s="14" t="str">
-        <f>INVCOST!C39</f>
+        <f>INVCOST!C40</f>
         <v>T-CAR-ICE_NGB21</v>
       </c>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14">
-        <f>INVCOST!G39</f>
-        <v>2030</v>
+        <f>INVCOST!G40</f>
+        <v>2050</v>
       </c>
       <c r="H55" s="14"/>
       <c r="I55" s="14" t="str">
-        <f>INVCOST!I39</f>
+        <f>INVCOST!I40</f>
         <v>EUR18</v>
       </c>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
       <c r="L55" s="44">
-        <f>INVCOST!L39*$C$3+IF(NOT(ISERR(FIND($B$8,C55))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C55))),$C$7,0)</f>
+        <f>INVCOST!L40*$C$3+IF(NOT(ISERR(FIND($B$8,C55))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C55))),$C$7,0)</f>
         <v>28.079339999999998</v>
       </c>
       <c r="O55" s="14"/>
@@ -10757,26 +10773,26 @@
         <v>177</v>
       </c>
       <c r="C56" s="14" t="str">
-        <f>INVCOST!C40</f>
-        <v>T-CAR-ICE_NGB21</v>
+        <f>INVCOST!C41</f>
+        <v>T-CAR-PHEV10_DST21</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
       <c r="G56" s="14">
-        <f>INVCOST!G40</f>
-        <v>2050</v>
+        <f>INVCOST!G41</f>
+        <v>2018</v>
       </c>
       <c r="H56" s="14"/>
       <c r="I56" s="14" t="str">
-        <f>INVCOST!I40</f>
+        <f>INVCOST!I41</f>
         <v>EUR18</v>
       </c>
       <c r="J56" s="14"/>
       <c r="K56" s="14"/>
       <c r="L56" s="44">
-        <f>INVCOST!L40*$C$3+IF(NOT(ISERR(FIND($B$8,C56))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C56))),$C$7,0)</f>
-        <v>28.079339999999998</v>
+        <f>INVCOST!L41*$C$3+IF(NOT(ISERR(FIND($B$8,C56))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C56))),$C$7,0)</f>
+        <v>35.602789999999992</v>
       </c>
       <c r="O56" s="14"/>
     </row>
@@ -10785,26 +10801,26 @@
         <v>177</v>
       </c>
       <c r="C57" s="14" t="str">
-        <f>INVCOST!C41</f>
+        <f>INVCOST!C42</f>
         <v>T-CAR-PHEV10_DST21</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14">
-        <f>INVCOST!G41</f>
-        <v>2018</v>
+        <f>INVCOST!G42</f>
+        <v>2030</v>
       </c>
       <c r="H57" s="14"/>
       <c r="I57" s="14" t="str">
-        <f>INVCOST!I41</f>
+        <f>INVCOST!I42</f>
         <v>EUR18</v>
       </c>
       <c r="J57" s="14"/>
       <c r="K57" s="14"/>
       <c r="L57" s="44">
-        <f>INVCOST!L41*$C$3+IF(NOT(ISERR(FIND($B$8,C57))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C57))),$C$7,0)</f>
-        <v>35.602789999999992</v>
+        <f>INVCOST!L42*$C$3+IF(NOT(ISERR(FIND($B$8,C57))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C57))),$C$7,0)</f>
+        <v>30.502999999999993</v>
       </c>
       <c r="O57" s="14"/>
     </row>
@@ -10813,26 +10829,26 @@
         <v>177</v>
       </c>
       <c r="C58" s="14" t="str">
-        <f>INVCOST!C42</f>
+        <f>INVCOST!C43</f>
         <v>T-CAR-PHEV10_DST21</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14">
-        <f>INVCOST!G42</f>
-        <v>2030</v>
+        <f>INVCOST!G43</f>
+        <v>2050</v>
       </c>
       <c r="H58" s="14"/>
       <c r="I58" s="14" t="str">
-        <f>INVCOST!I42</f>
+        <f>INVCOST!I43</f>
         <v>EUR18</v>
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="14"/>
       <c r="L58" s="44">
-        <f>INVCOST!L42*$C$3+IF(NOT(ISERR(FIND($B$8,C58))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C58))),$C$7,0)</f>
-        <v>30.502999999999993</v>
+        <f>INVCOST!L43*$C$3+IF(NOT(ISERR(FIND($B$8,C58))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C58))),$C$7,0)</f>
+        <v>28.709779999999995</v>
       </c>
       <c r="O58" s="14"/>
     </row>
@@ -10841,26 +10857,26 @@
         <v>177</v>
       </c>
       <c r="C59" s="14" t="str">
-        <f>INVCOST!C43</f>
-        <v>T-CAR-PHEV10_DST21</v>
+        <f>INVCOST!C44</f>
+        <v>T-CAR-PHEV10_GSL21</v>
       </c>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14">
-        <f>INVCOST!G43</f>
-        <v>2050</v>
+        <f>INVCOST!G44</f>
+        <v>2018</v>
       </c>
       <c r="H59" s="14"/>
       <c r="I59" s="14" t="str">
-        <f>INVCOST!I43</f>
+        <f>INVCOST!I44</f>
         <v>EUR18</v>
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="14"/>
       <c r="L59" s="44">
-        <f>INVCOST!L43*$C$3+IF(NOT(ISERR(FIND($B$8,C59))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C59))),$C$7,0)</f>
-        <v>28.709779999999995</v>
+        <f>INVCOST!L44*$C$3+IF(NOT(ISERR(FIND($B$8,C59))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C59))),$C$7,0)</f>
+        <v>32.782429999999998</v>
       </c>
       <c r="O59" s="14"/>
     </row>
@@ -10869,26 +10885,26 @@
         <v>177</v>
       </c>
       <c r="C60" s="14" t="str">
-        <f>INVCOST!C44</f>
+        <f>INVCOST!C45</f>
         <v>T-CAR-PHEV10_GSL21</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14">
-        <f>INVCOST!G44</f>
-        <v>2018</v>
+        <f>INVCOST!G45</f>
+        <v>2030</v>
       </c>
       <c r="H60" s="14"/>
       <c r="I60" s="14" t="str">
-        <f>INVCOST!I44</f>
+        <f>INVCOST!I45</f>
         <v>EUR18</v>
       </c>
       <c r="J60" s="14"/>
       <c r="K60" s="14"/>
       <c r="L60" s="44">
-        <f>INVCOST!L44*$C$3+IF(NOT(ISERR(FIND($B$8,C60))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C60))),$C$7,0)</f>
-        <v>32.782429999999998</v>
+        <f>INVCOST!L45*$C$3+IF(NOT(ISERR(FIND($B$8,C60))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C60))),$C$7,0)</f>
+        <v>28.085059999999999</v>
       </c>
       <c r="O60" s="14"/>
     </row>
@@ -10897,26 +10913,26 @@
         <v>177</v>
       </c>
       <c r="C61" s="14" t="str">
-        <f>INVCOST!C45</f>
+        <f>INVCOST!C46</f>
         <v>T-CAR-PHEV10_GSL21</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14">
-        <f>INVCOST!G45</f>
-        <v>2030</v>
+        <f>INVCOST!G46</f>
+        <v>2050</v>
       </c>
       <c r="H61" s="14"/>
       <c r="I61" s="14" t="str">
-        <f>INVCOST!I45</f>
+        <f>INVCOST!I46</f>
         <v>EUR18</v>
       </c>
       <c r="J61" s="14"/>
       <c r="K61" s="14"/>
       <c r="L61" s="44">
-        <f>INVCOST!L45*$C$3+IF(NOT(ISERR(FIND($B$8,C61))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C61))),$C$7,0)</f>
-        <v>28.085059999999999</v>
+        <f>INVCOST!L46*$C$3+IF(NOT(ISERR(FIND($B$8,C61))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C61))),$C$7,0)</f>
+        <v>26.422939999999997</v>
       </c>
       <c r="O61" s="14"/>
     </row>
@@ -10925,26 +10941,26 @@
         <v>177</v>
       </c>
       <c r="C62" s="14" t="str">
-        <f>INVCOST!C46</f>
-        <v>T-CAR-PHEV10_GSL21</v>
+        <f>INVCOST!C47</f>
+        <v>T-CAR-PHEV20_DST21</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14">
-        <f>INVCOST!G46</f>
-        <v>2050</v>
+        <f>INVCOST!G47</f>
+        <v>2018</v>
       </c>
       <c r="H62" s="14"/>
       <c r="I62" s="14" t="str">
-        <f>INVCOST!I46</f>
+        <f>INVCOST!I47</f>
         <v>EUR18</v>
       </c>
       <c r="J62" s="14"/>
       <c r="K62" s="14"/>
       <c r="L62" s="44">
-        <f>INVCOST!L46*$C$3+IF(NOT(ISERR(FIND($B$8,C62))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C62))),$C$7,0)</f>
-        <v>26.422939999999997</v>
+        <f>INVCOST!L47*$C$3+IF(NOT(ISERR(FIND($B$8,C62))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C62))),$C$7,0)</f>
+        <v>35.602789999999992</v>
       </c>
       <c r="O62" s="14"/>
     </row>
@@ -10953,26 +10969,26 @@
         <v>177</v>
       </c>
       <c r="C63" s="14" t="str">
-        <f>INVCOST!C47</f>
+        <f>INVCOST!C48</f>
         <v>T-CAR-PHEV20_DST21</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14">
-        <f>INVCOST!G47</f>
-        <v>2018</v>
+        <f>INVCOST!G48</f>
+        <v>2030</v>
       </c>
       <c r="H63" s="14"/>
       <c r="I63" s="14" t="str">
-        <f>INVCOST!I47</f>
+        <f>INVCOST!I48</f>
         <v>EUR18</v>
       </c>
       <c r="J63" s="14"/>
       <c r="K63" s="14"/>
       <c r="L63" s="44">
-        <f>INVCOST!L47*$C$3+IF(NOT(ISERR(FIND($B$8,C63))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C63))),$C$7,0)</f>
-        <v>35.602789999999992</v>
+        <f>INVCOST!L48*$C$3+IF(NOT(ISERR(FIND($B$8,C63))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C63))),$C$7,0)</f>
+        <v>30.502999999999993</v>
       </c>
       <c r="O63" s="14"/>
     </row>
@@ -10981,26 +10997,26 @@
         <v>177</v>
       </c>
       <c r="C64" s="14" t="str">
-        <f>INVCOST!C48</f>
+        <f>INVCOST!C49</f>
         <v>T-CAR-PHEV20_DST21</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
       <c r="G64" s="14">
-        <f>INVCOST!G48</f>
-        <v>2030</v>
+        <f>INVCOST!G49</f>
+        <v>2050</v>
       </c>
       <c r="H64" s="14"/>
       <c r="I64" s="14" t="str">
-        <f>INVCOST!I48</f>
+        <f>INVCOST!I49</f>
         <v>EUR18</v>
       </c>
       <c r="J64" s="14"/>
       <c r="K64" s="14"/>
       <c r="L64" s="44">
-        <f>INVCOST!L48*$C$3+IF(NOT(ISERR(FIND($B$8,C64))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C64))),$C$7,0)</f>
-        <v>30.502999999999993</v>
+        <f>INVCOST!L49*$C$3+IF(NOT(ISERR(FIND($B$8,C64))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C64))),$C$7,0)</f>
+        <v>28.709779999999995</v>
       </c>
       <c r="O64" s="14"/>
     </row>
@@ -11009,26 +11025,26 @@
         <v>177</v>
       </c>
       <c r="C65" s="14" t="str">
-        <f>INVCOST!C49</f>
-        <v>T-CAR-PHEV20_DST21</v>
+        <f>INVCOST!C50</f>
+        <v>T-CAR-PHEV20_GSL21</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
       <c r="G65" s="14">
-        <f>INVCOST!G49</f>
-        <v>2050</v>
+        <f>INVCOST!G50</f>
+        <v>2018</v>
       </c>
       <c r="H65" s="14"/>
       <c r="I65" s="14" t="str">
-        <f>INVCOST!I49</f>
+        <f>INVCOST!I50</f>
         <v>EUR18</v>
       </c>
       <c r="J65" s="14"/>
       <c r="K65" s="14"/>
       <c r="L65" s="44">
-        <f>INVCOST!L49*$C$3+IF(NOT(ISERR(FIND($B$8,C65))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C65))),$C$7,0)</f>
-        <v>28.709779999999995</v>
+        <f>INVCOST!L50*$C$3+IF(NOT(ISERR(FIND($B$8,C65))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C65))),$C$7,0)</f>
+        <v>32.782429999999998</v>
       </c>
       <c r="O65" s="14"/>
     </row>
@@ -11037,26 +11053,26 @@
         <v>177</v>
       </c>
       <c r="C66" s="14" t="str">
-        <f>INVCOST!C50</f>
+        <f>INVCOST!C51</f>
         <v>T-CAR-PHEV20_GSL21</v>
       </c>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
       <c r="G66" s="14">
-        <f>INVCOST!G50</f>
-        <v>2018</v>
+        <f>INVCOST!G51</f>
+        <v>2030</v>
       </c>
       <c r="H66" s="14"/>
       <c r="I66" s="14" t="str">
-        <f>INVCOST!I50</f>
+        <f>INVCOST!I51</f>
         <v>EUR18</v>
       </c>
       <c r="J66" s="14"/>
       <c r="K66" s="14"/>
       <c r="L66" s="44">
-        <f>INVCOST!L50*$C$3+IF(NOT(ISERR(FIND($B$8,C66))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C66))),$C$7,0)</f>
-        <v>32.782429999999998</v>
+        <f>INVCOST!L51*$C$3+IF(NOT(ISERR(FIND($B$8,C66))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C66))),$C$7,0)</f>
+        <v>28.085059999999999</v>
       </c>
       <c r="O66" s="14"/>
     </row>
@@ -11065,26 +11081,26 @@
         <v>177</v>
       </c>
       <c r="C67" s="14" t="str">
-        <f>INVCOST!C51</f>
+        <f>INVCOST!C52</f>
         <v>T-CAR-PHEV20_GSL21</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14">
-        <f>INVCOST!G51</f>
-        <v>2030</v>
+        <f>INVCOST!G52</f>
+        <v>2050</v>
       </c>
       <c r="H67" s="14"/>
       <c r="I67" s="14" t="str">
-        <f>INVCOST!I51</f>
+        <f>INVCOST!I52</f>
         <v>EUR18</v>
       </c>
       <c r="J67" s="14"/>
       <c r="K67" s="14"/>
       <c r="L67" s="44">
-        <f>INVCOST!L51*$C$3+IF(NOT(ISERR(FIND($B$8,C67))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C67))),$C$7,0)</f>
-        <v>28.085059999999999</v>
+        <f>INVCOST!L52*$C$3+IF(NOT(ISERR(FIND($B$8,C67))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C67))),$C$7,0)</f>
+        <v>26.422939999999997</v>
       </c>
       <c r="O67" s="14"/>
     </row>
@@ -11093,26 +11109,26 @@
         <v>177</v>
       </c>
       <c r="C68" s="14" t="str">
-        <f>INVCOST!C52</f>
-        <v>T-CAR-PHEV20_GSL21</v>
+        <f>INVCOST!C53</f>
+        <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14">
-        <f>INVCOST!G52</f>
-        <v>2050</v>
+        <f>INVCOST!G53</f>
+        <v>2018</v>
       </c>
       <c r="H68" s="14"/>
       <c r="I68" s="14" t="str">
-        <f>INVCOST!I52</f>
+        <f>INVCOST!I53</f>
         <v>EUR18</v>
       </c>
       <c r="J68" s="14"/>
       <c r="K68" s="14"/>
       <c r="L68" s="44">
-        <f>INVCOST!L52*$C$3+IF(NOT(ISERR(FIND($B$8,C68))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C68))),$C$7,0)</f>
-        <v>26.422939999999997</v>
+        <f>INVCOST!L53*$C$3+IF(NOT(ISERR(FIND($B$8,C68))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C68))),$C$7,0)</f>
+        <v>35.602789999999992</v>
       </c>
       <c r="O68" s="14"/>
     </row>
@@ -11121,26 +11137,26 @@
         <v>177</v>
       </c>
       <c r="C69" s="14" t="str">
-        <f>INVCOST!C53</f>
+        <f>INVCOST!C54</f>
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14">
-        <f>INVCOST!G53</f>
-        <v>2018</v>
+        <f>INVCOST!G54</f>
+        <v>2030</v>
       </c>
       <c r="H69" s="14"/>
       <c r="I69" s="14" t="str">
-        <f>INVCOST!I53</f>
+        <f>INVCOST!I54</f>
         <v>EUR18</v>
       </c>
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
       <c r="L69" s="44">
-        <f>INVCOST!L53*$C$3+IF(NOT(ISERR(FIND($B$8,C69))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C69))),$C$7,0)</f>
-        <v>35.602789999999992</v>
+        <f>INVCOST!L54*$C$3+IF(NOT(ISERR(FIND($B$8,C69))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C69))),$C$7,0)</f>
+        <v>30.502999999999993</v>
       </c>
       <c r="O69" s="14"/>
     </row>
@@ -11149,26 +11165,26 @@
         <v>177</v>
       </c>
       <c r="C70" s="14" t="str">
-        <f>INVCOST!C54</f>
+        <f>INVCOST!C55</f>
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
       <c r="G70" s="14">
-        <f>INVCOST!G54</f>
-        <v>2030</v>
+        <f>INVCOST!G55</f>
+        <v>2050</v>
       </c>
       <c r="H70" s="14"/>
       <c r="I70" s="14" t="str">
-        <f>INVCOST!I54</f>
+        <f>INVCOST!I55</f>
         <v>EUR18</v>
       </c>
       <c r="J70" s="14"/>
       <c r="K70" s="14"/>
       <c r="L70" s="44">
-        <f>INVCOST!L54*$C$3+IF(NOT(ISERR(FIND($B$8,C70))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C70))),$C$7,0)</f>
-        <v>30.502999999999993</v>
+        <f>INVCOST!L55*$C$3+IF(NOT(ISERR(FIND($B$8,C70))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C70))),$C$7,0)</f>
+        <v>28.709779999999995</v>
       </c>
       <c r="O70" s="14"/>
     </row>
@@ -11177,26 +11193,26 @@
         <v>177</v>
       </c>
       <c r="C71" s="14" t="str">
-        <f>INVCOST!C55</f>
-        <v>T-CAR-PHEV40_DST21</v>
+        <f>INVCOST!C56</f>
+        <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
       <c r="G71" s="14">
-        <f>INVCOST!G55</f>
-        <v>2050</v>
+        <f>INVCOST!G56</f>
+        <v>2018</v>
       </c>
       <c r="H71" s="14"/>
       <c r="I71" s="14" t="str">
-        <f>INVCOST!I55</f>
+        <f>INVCOST!I56</f>
         <v>EUR18</v>
       </c>
       <c r="J71" s="14"/>
       <c r="K71" s="14"/>
       <c r="L71" s="44">
-        <f>INVCOST!L55*$C$3+IF(NOT(ISERR(FIND($B$8,C71))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C71))),$C$7,0)</f>
-        <v>28.709779999999995</v>
+        <f>INVCOST!L56*$C$3+IF(NOT(ISERR(FIND($B$8,C71))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C71))),$C$7,0)</f>
+        <v>32.782429999999998</v>
       </c>
       <c r="O71" s="14"/>
     </row>
@@ -11205,26 +11221,26 @@
         <v>177</v>
       </c>
       <c r="C72" s="14" t="str">
-        <f>INVCOST!C56</f>
+        <f>INVCOST!C57</f>
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
       <c r="G72" s="14">
-        <f>INVCOST!G56</f>
-        <v>2018</v>
+        <f>INVCOST!G57</f>
+        <v>2030</v>
       </c>
       <c r="H72" s="14"/>
       <c r="I72" s="14" t="str">
-        <f>INVCOST!I56</f>
+        <f>INVCOST!I57</f>
         <v>EUR18</v>
       </c>
       <c r="J72" s="14"/>
       <c r="K72" s="14"/>
       <c r="L72" s="44">
-        <f>INVCOST!L56*$C$3+IF(NOT(ISERR(FIND($B$8,C72))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C72))),$C$7,0)</f>
-        <v>32.782429999999998</v>
+        <f>INVCOST!L57*$C$3+IF(NOT(ISERR(FIND($B$8,C72))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C72))),$C$7,0)</f>
+        <v>28.085059999999999</v>
       </c>
       <c r="O72" s="14"/>
     </row>
@@ -11233,56 +11249,41 @@
         <v>177</v>
       </c>
       <c r="C73" s="14" t="str">
-        <f>INVCOST!C57</f>
+        <f>INVCOST!C58</f>
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14">
-        <f>INVCOST!G57</f>
-        <v>2030</v>
+        <f>INVCOST!G58</f>
+        <v>2050</v>
       </c>
       <c r="H73" s="14"/>
       <c r="I73" s="14" t="str">
-        <f>INVCOST!I57</f>
+        <f>INVCOST!I58</f>
         <v>EUR18</v>
       </c>
       <c r="J73" s="14"/>
       <c r="K73" s="14"/>
       <c r="L73" s="44">
-        <f>INVCOST!L57*$C$3+IF(NOT(ISERR(FIND($B$8,C73))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C73))),$C$7,0)</f>
-        <v>28.085059999999999</v>
+        <f>INVCOST!L58*$C$3+IF(NOT(ISERR(FIND($B$8,C73))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C73))),$C$7,0)</f>
+        <v>26.422939999999997</v>
       </c>
       <c r="O73" s="14"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B74" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C74" s="14" t="str">
-        <f>INVCOST!C58</f>
-        <v>T-CAR-PHEV40_GSL21</v>
-      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
-      <c r="G74" s="14">
-        <f>INVCOST!G58</f>
-        <v>2050</v>
-      </c>
+      <c r="G74" s="14"/>
       <c r="H74" s="14"/>
-      <c r="I74" s="14" t="str">
-        <f>INVCOST!I58</f>
-        <v>EUR18</v>
-      </c>
+      <c r="I74" s="14"/>
       <c r="J74" s="14"/>
       <c r="K74" s="14"/>
-      <c r="L74" s="44">
-        <f>INVCOST!L58*$C$3+IF(NOT(ISERR(FIND($B$8,C74))),$C$8,0)+IF(NOT(ISERR(FIND($B$7,C74))),$C$7,0)</f>
-        <v>26.422939999999997</v>
-      </c>
-      <c r="O74" s="14"/>
+      <c r="L74" s="44"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B75" s="14"/>
@@ -11491,19 +11492,6 @@
       <c r="J90" s="14"/>
       <c r="K90" s="14"/>
       <c r="L90" s="44"/>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="44"/>
     </row>
   </sheetData>
   <phoneticPr fontId="25" type="noConversion"/>

</xml_diff>